<commit_message>
feat: cf tracker updates
</commit_message>
<xml_diff>
--- a/trackers-and-planning/cloud-foundations-tracker/Cloud Foundations Tracker.xlsx
+++ b/trackers-and-planning/cloud-foundations-tracker/Cloud Foundations Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awstodd/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awstodd/unCode/Gits/GITHUB-CloudFoundations/cloud-foundations-templates/trackers-and-planning/cloud-foundations-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81B5C18F-8243-6940-92F1-AEB354876859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B1A540-EC60-8C48-920B-FA158FA00823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52500" yWindow="500" windowWidth="49060" windowHeight="23340" xr2:uid="{8357623D-2B7C-8445-9F5B-200FB7F3C4BA}"/>
+    <workbookView xWindow="52500" yWindow="500" windowWidth="49060" windowHeight="23340" activeTab="1" xr2:uid="{8357623D-2B7C-8445-9F5B-200FB7F3C4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="396">
   <si>
     <t>Customer Name</t>
   </si>
@@ -809,24 +809,12 @@
     <t>Patch rollback and recovery</t>
   </si>
   <si>
-    <t>Assess and identify vulnerabilities</t>
-  </si>
-  <si>
-    <t>Respond to vulnerabilities</t>
-  </si>
-  <si>
-    <t>Report on vulnerabilties</t>
-  </si>
-  <si>
     <t>CF7-S5</t>
   </si>
   <si>
     <t>CF8-S5</t>
   </si>
   <si>
-    <t>Design isolated resource environments</t>
-  </si>
-  <si>
     <t>Isolated environment lifecycle management</t>
   </si>
   <si>
@@ -944,12 +932,6 @@
     <t>Evidence reporting</t>
   </si>
   <si>
-    <t>Classify and prioritize vulnerabilities</t>
-  </si>
-  <si>
-    <t>Improve process</t>
-  </si>
-  <si>
     <t>Repeatable patterns for isolated enviornments</t>
   </si>
   <si>
@@ -1070,18 +1052,12 @@
     <t>Change Management Fulfillment</t>
   </si>
   <si>
-    <t>Change Rollback</t>
-  </si>
-  <si>
     <t>Change Monitoring and Assessment</t>
   </si>
   <si>
     <t>Stakeholders</t>
   </si>
   <si>
-    <t>Coming Soon</t>
-  </si>
-  <si>
     <t>Backup requirements and strategy</t>
   </si>
   <si>
@@ -1173,6 +1149,81 @@
   </si>
   <si>
     <t>Compliance management</t>
+  </si>
+  <si>
+    <t>CF31</t>
+  </si>
+  <si>
+    <t>Image Management</t>
+  </si>
+  <si>
+    <t>CF31-S1</t>
+  </si>
+  <si>
+    <t>CF31-S2</t>
+  </si>
+  <si>
+    <t>CF31-S3</t>
+  </si>
+  <si>
+    <t>Image development</t>
+  </si>
+  <si>
+    <t>Image storage and distribution</t>
+  </si>
+  <si>
+    <t>Image lifecycle management</t>
+  </si>
+  <si>
+    <t>Change Rollout/Rollback</t>
+  </si>
+  <si>
+    <t>Support requirements and strategy</t>
+  </si>
+  <si>
+    <t>Ticketing system(s) and integration</t>
+  </si>
+  <si>
+    <t>Support and operational readiness</t>
+  </si>
+  <si>
+    <t>Health monitoring</t>
+  </si>
+  <si>
+    <t>CF12-S5</t>
+  </si>
+  <si>
+    <t>CF12-S6</t>
+  </si>
+  <si>
+    <t>Operational event management</t>
+  </si>
+  <si>
+    <t>Environment access for support</t>
+  </si>
+  <si>
+    <t>CF10-S5</t>
+  </si>
+  <si>
+    <t>Data residency</t>
+  </si>
+  <si>
+    <t>Designing isolated resource environments</t>
+  </si>
+  <si>
+    <t>Process improvement</t>
+  </si>
+  <si>
+    <t>Vulnerability identification and assessment</t>
+  </si>
+  <si>
+    <t>Vulnerability classification and prioritization</t>
+  </si>
+  <si>
+    <t>Vulnerability response</t>
+  </si>
+  <si>
+    <t>Vulnerability reporting</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1586,13 +1637,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -1602,162 +1646,53 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF010022"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF010022"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF010022"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF010022"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF010022"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF010022"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF010022"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF010022"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2089,11 +2024,143 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF010022"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF010022"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF010022"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF010022"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF010022"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF010022"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF010022"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF010022"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF010022"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2180,32 +2247,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C32B6F1C-594B-EF46-9E98-D6C31AE3F5ED}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C32B6F1C-594B-EF46-9E98-D6C31AE3F5ED}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:C8" xr:uid="{458A2142-5A50-7D4E-8042-7BD4B32DCDCE}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3C316A9B-7332-4349-AAA4-7238D66CC0CA}" name="Question" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{7C60BFEC-A699-8843-9E5F-DBE547E55959}" name="Answer" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{329AD68F-C5D6-9A4D-AF8C-830676506BC8}" name="Instructions" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3C316A9B-7332-4349-AAA4-7238D66CC0CA}" name="Question" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7C60BFEC-A699-8843-9E5F-DBE547E55959}" name="Answer" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{329AD68F-C5D6-9A4D-AF8C-830676506BC8}" name="Instructions" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}" name="Table2" displayName="Table2" ref="A2:K150" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A2:K150" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}" name="Table2" displayName="Table2" ref="A2:K157" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K157" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FE1167A3-DF76-D74B-B521-E68F0EB60494}" name="CAP ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{6407AEF3-7924-094D-8A5A-40B9D718CCE6}" name="Scenario ID" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{A748EA53-7C5A-7B4D-87B7-4CB9B473475D}" name="Capability" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{55B54472-AD4E-8445-B71E-3AE1E9AC463C}" name="Scenario" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{573429BF-70FF-C746-8240-F6FD8088D7C8}" name="Stakeholders" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{BF4B01D1-8572-4143-B02F-99490778142C}" name="Completed" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{FDBC1E55-1B33-C64A-A2C1-6432DD8F973F}" name="Stage" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{B1CF695B-93BA-EF4B-BD07-B17D64F157F9}" name="Notes" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{8EAD3560-DBF5-1941-BA7D-9D7E3F958354}" name="Owner" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{F0BC2494-A3E4-8443-A2EF-E1DCC2C91ABE}" name="Feedback" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{EECFCACA-6655-204B-9A4E-DB5D71ED9602}" name="Time to completion (in weeks)" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{FE1167A3-DF76-D74B-B521-E68F0EB60494}" name="CAP ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6407AEF3-7924-094D-8A5A-40B9D718CCE6}" name="Scenario ID" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{A748EA53-7C5A-7B4D-87B7-4CB9B473475D}" name="Capability" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{55B54472-AD4E-8445-B71E-3AE1E9AC463C}" name="Scenario" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{573429BF-70FF-C746-8240-F6FD8088D7C8}" name="Stakeholders" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BF4B01D1-8572-4143-B02F-99490778142C}" name="Completed" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FDBC1E55-1B33-C64A-A2C1-6432DD8F973F}" name="Stage" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{B1CF695B-93BA-EF4B-BD07-B17D64F157F9}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{8EAD3560-DBF5-1941-BA7D-9D7E3F958354}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{F0BC2494-A3E4-8443-A2EF-E1DCC2C91ABE}" name="Feedback" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{EECFCACA-6655-204B-9A4E-DB5D71ED9602}" name="Time to completion (in weeks)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2510,7 +2577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A01F414-5472-0445-9FF4-8BCF3433CDD1}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="224" workbookViewId="0">
+    <sheetView zoomScale="224" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2522,76 +2589,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="45" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="44" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44" t="s">
-        <v>372</v>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2599,8 +2666,8 @@
       <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="2">
-        <f>COUNTIF(Capabilities!$F$3:$F$150,"Yes")</f>
+      <c r="B11" s="54">
+        <f>COUNTIF(Capabilities!$F$3:$F$157,"Yes")</f>
         <v>0</v>
       </c>
     </row>
@@ -2656,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0651646F-D6FF-204E-8928-F8B104176F10}">
-  <dimension ref="A1:K150"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2677,21 +2744,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
-        <v>369</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39" t="s">
-        <v>370</v>
-      </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
+      <c r="A1" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48" t="s">
+        <v>362</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -2707,7 +2774,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>64</v>
@@ -2789,7 +2856,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>84</v>
@@ -2815,7 +2882,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>84</v>
@@ -2889,7 +2956,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>67</v>
@@ -2914,7 +2981,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>67</v>
@@ -2933,13 +3000,13 @@
         <v>120</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>67</v>
@@ -3012,7 +3079,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>67</v>
@@ -3160,7 +3227,7 @@
         <v>56</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>67</v>
@@ -3210,7 +3277,7 @@
         <v>56</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>67</v>
@@ -3230,7 +3297,7 @@
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="24" t="s">
@@ -3255,7 +3322,7 @@
         <v>146</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>252</v>
@@ -3280,7 +3347,7 @@
         <v>156</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>253</v>
@@ -3305,7 +3372,7 @@
         <v>157</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>254</v>
@@ -3330,7 +3397,7 @@
         <v>158</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>255</v>
@@ -3355,7 +3422,7 @@
         <v>159</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>256</v>
@@ -3406,7 +3473,7 @@
         <v>60</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>257</v>
+        <v>392</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>67</v>
@@ -3431,7 +3498,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>302</v>
+        <v>393</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>67</v>
@@ -3456,7 +3523,7 @@
         <v>60</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>258</v>
+        <v>394</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>67</v>
@@ -3481,7 +3548,7 @@
         <v>60</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>259</v>
+        <v>395</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>67</v>
@@ -3506,7 +3573,7 @@
         <v>60</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>303</v>
+        <v>391</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>67</v>
@@ -3548,13 +3615,13 @@
         <v>125</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>262</v>
+        <v>390</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>86</v>
@@ -3573,13 +3640,13 @@
         <v>125</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>86</v>
@@ -3598,13 +3665,13 @@
         <v>125</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>86</v>
@@ -3623,13 +3690,13 @@
         <v>125</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>86</v>
@@ -3677,7 +3744,7 @@
         <v>57</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>87</v>
@@ -3702,7 +3769,7 @@
         <v>57</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>87</v>
@@ -3727,7 +3794,7 @@
         <v>57</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>87</v>
@@ -3752,7 +3819,7 @@
         <v>57</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>87</v>
@@ -3771,13 +3838,13 @@
         <v>126</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>87</v>
@@ -3825,7 +3892,7 @@
         <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>88</v>
@@ -3850,7 +3917,7 @@
         <v>46</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>88</v>
@@ -3875,7 +3942,7 @@
         <v>46</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>88</v>
@@ -3900,7 +3967,7 @@
         <v>46</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>88</v>
@@ -3948,7 +4015,7 @@
         <v>44</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>88</v>
@@ -3973,7 +4040,7 @@
         <v>44</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>88</v>
@@ -3998,7 +4065,7 @@
         <v>44</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>88</v>
@@ -4023,7 +4090,7 @@
         <v>44</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>88</v>
@@ -4037,66 +4104,66 @@
       <c r="J55" s="13"/>
       <c r="K55" s="14"/>
     </row>
-    <row r="56" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="53"/>
+    </row>
+    <row r="57" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22" t="s">
+      <c r="B57" s="22"/>
+      <c r="C57" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="24" t="s">
+      <c r="D57" s="23"/>
+      <c r="E57" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="F56" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G56" s="26" t="s">
+      <c r="F57" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G57" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="27"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="14"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="27"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>89</v>
@@ -4115,13 +4182,13 @@
         <v>111</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>89</v>
@@ -4140,13 +4207,13 @@
         <v>111</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>89</v>
@@ -4165,13 +4232,13 @@
         <v>111</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>285</v>
+        <v>188</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>89</v>
@@ -4190,15 +4257,15 @@
         <v>111</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E62" s="7" t="s">
+      <c r="D62" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F62" s="12" t="s">
@@ -4210,66 +4277,66 @@
       <c r="J62" s="13"/>
       <c r="K62" s="14"/>
     </row>
-    <row r="63" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="14"/>
+    </row>
+    <row r="64" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22" t="s">
+      <c r="B64" s="22"/>
+      <c r="C64" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D63" s="23"/>
-      <c r="E63" s="24" t="s">
+      <c r="D64" s="23"/>
+      <c r="E64" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F63" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G63" s="26" t="s">
+      <c r="F64" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G64" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H63" s="25"/>
-      <c r="I63" s="25"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="27"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F64" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="14"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="27"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>90</v>
@@ -4288,13 +4355,13 @@
         <v>112</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>90</v>
@@ -4313,13 +4380,13 @@
         <v>112</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>90</v>
@@ -4333,147 +4400,149 @@
       <c r="J67" s="13"/>
       <c r="K67" s="14"/>
     </row>
-    <row r="68" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="22" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="14"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="49" t="s">
+        <v>386</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G69" s="52"/>
+      <c r="H69" s="52"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="53"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="49" t="s">
+        <v>385</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="49" t="s">
+        <v>387</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G70" s="52"/>
+      <c r="H70" s="52"/>
+      <c r="I70" s="51"/>
+      <c r="J70" s="52"/>
+      <c r="K70" s="53"/>
+    </row>
+    <row r="71" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22" t="s">
+      <c r="B71" s="22"/>
+      <c r="C71" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="23"/>
-      <c r="E68" s="24" t="s">
+      <c r="D71" s="23"/>
+      <c r="E71" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="F68" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G68" s="26" t="s">
+      <c r="F71" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H68" s="25"/>
-      <c r="I68" s="25"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="27"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="H71" s="25"/>
+      <c r="I71" s="25"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="27"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B72" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="E69" s="6" t="s">
+      <c r="D72" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F69" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F70" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F71" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-    </row>
-    <row r="72" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="D72" s="23"/>
-      <c r="E72" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F72" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G72" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H72" s="25"/>
-      <c r="I72" s="25"/>
-      <c r="J72" s="26"/>
-      <c r="K72" s="27"/>
+      <c r="F72" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G73" s="19"/>
+        <v>301</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F73" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G73" s="13"/>
       <c r="H73" s="13"/>
       <c r="I73" s="12"/>
       <c r="J73" s="13"/>
@@ -4481,66 +4550,64 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F74" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G74" s="19"/>
+        <v>284</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G74" s="13"/>
       <c r="H74" s="13"/>
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
-      <c r="K74" s="16"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
+      <c r="K74" s="13"/>
+    </row>
+    <row r="75" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="E75" s="4" t="s">
+      <c r="B75" s="22"/>
+      <c r="C75" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="F75" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G75" s="19"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="16"/>
+      <c r="F75" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G75" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H75" s="25"/>
+      <c r="I75" s="25"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="27"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>91</v>
@@ -4552,20 +4619,20 @@
       <c r="H76" s="13"/>
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
-      <c r="K76" s="16"/>
+      <c r="K76" s="13"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>91</v>
@@ -4584,13 +4651,13 @@
         <v>106</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>368</v>
+        <v>304</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>91</v>
@@ -4604,44 +4671,46 @@
       <c r="J78" s="13"/>
       <c r="K78" s="16"/>
     </row>
-    <row r="79" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A79" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B79" s="22"/>
-      <c r="C79" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D79" s="23"/>
-      <c r="E79" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F79" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G79" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H79" s="25"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="26"/>
-      <c r="K79" s="27"/>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G79" s="19"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="16"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>182</v>
+        <v>240</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>107</v>
+        <v>359</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>83</v>
@@ -4654,19 +4723,19 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>107</v>
+        <v>359</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>313</v>
+        <v>360</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F81" s="18" t="s">
         <v>83</v>
@@ -4677,43 +4746,41 @@
       <c r="J81" s="13"/>
       <c r="K81" s="16"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+    <row r="82" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C82" s="5" t="s">
+      <c r="B82" s="22"/>
+      <c r="C82" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D82" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E82" s="4" t="s">
+      <c r="D82" s="23"/>
+      <c r="E82" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="F82" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G82" s="19"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="16"/>
+      <c r="F82" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G82" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H82" s="25"/>
+      <c r="I82" s="25"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="27"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>107</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>92</v>
@@ -4732,13 +4799,13 @@
         <v>108</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>107</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>92</v>
@@ -4752,116 +4819,116 @@
       <c r="J84" s="13"/>
       <c r="K84" s="16"/>
     </row>
-    <row r="85" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B85" s="22"/>
-      <c r="C85" s="22" t="s">
-        <v>317</v>
-      </c>
-      <c r="D85" s="23"/>
-      <c r="E85" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F85" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G85" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H85" s="25"/>
-      <c r="I85" s="25"/>
-      <c r="J85" s="26"/>
-      <c r="K85" s="27"/>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G85" s="19"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="16"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>317</v>
+        <v>107</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F86" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G86" s="13"/>
+        <v>92</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G86" s="19"/>
       <c r="H86" s="13"/>
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
+      <c r="K86" s="16"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>317</v>
+        <v>107</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>349</v>
+        <v>310</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F87" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G87" s="13"/>
+        <v>92</v>
+      </c>
+      <c r="F87" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G87" s="19"/>
       <c r="H87" s="13"/>
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
+      <c r="K87" s="16"/>
+    </row>
+    <row r="88" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="E88" s="4" t="s">
+      <c r="B88" s="22"/>
+      <c r="C88" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="D88" s="23"/>
+      <c r="E88" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="F88" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
+      <c r="F88" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G88" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="27"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>94</v>
@@ -4880,13 +4947,13 @@
         <v>113</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>290</v>
+        <v>202</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>94</v>
@@ -4900,44 +4967,46 @@
       <c r="J90" s="13"/>
       <c r="K90" s="13"/>
     </row>
-    <row r="91" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A91" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B91" s="22"/>
-      <c r="C91" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" s="23"/>
-      <c r="E91" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F91" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G91" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H91" s="25"/>
-      <c r="I91" s="25"/>
-      <c r="J91" s="26"/>
-      <c r="K91" s="27"/>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F91" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="13"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>50</v>
+        <v>311</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F92" s="12" t="s">
         <v>83</v>
@@ -4950,19 +5019,19 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>205</v>
+        <v>286</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>50</v>
+        <v>311</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F93" s="12" t="s">
         <v>83</v>
@@ -4973,69 +5042,69 @@
       <c r="J93" s="13"/>
       <c r="K93" s="13"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+    <row r="94" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="B94" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C94" s="5" t="s">
+      <c r="B94" s="22"/>
+      <c r="C94" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D94" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="E94" s="4" t="s">
+      <c r="D94" s="23"/>
+      <c r="E94" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="F94" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="12"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-    </row>
-    <row r="95" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A95" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B95" s="22"/>
-      <c r="C95" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D95" s="23"/>
-      <c r="E95" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F95" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G95" s="26" t="s">
+      <c r="F94" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G94" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H95" s="25"/>
-      <c r="I95" s="25"/>
-      <c r="J95" s="26"/>
-      <c r="K95" s="27"/>
+      <c r="H94" s="25"/>
+      <c r="I94" s="25"/>
+      <c r="J94" s="26"/>
+      <c r="K94" s="27"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="13"/>
+      <c r="K95" s="13"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>83</v>
@@ -5044,23 +5113,23 @@
       <c r="H96" s="13"/>
       <c r="I96" s="12"/>
       <c r="J96" s="13"/>
-      <c r="K96" s="14"/>
+      <c r="K96" s="13"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>291</v>
+        <v>347</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>83</v>
@@ -5069,45 +5138,43 @@
       <c r="H97" s="13"/>
       <c r="I97" s="12"/>
       <c r="J97" s="13"/>
-      <c r="K97" s="14"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
+      <c r="K97" s="13"/>
+    </row>
+    <row r="98" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C98" s="5" t="s">
+      <c r="B98" s="22"/>
+      <c r="C98" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="E98" s="4" t="s">
+      <c r="D98" s="23"/>
+      <c r="E98" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F98" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="12"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="14"/>
+      <c r="F98" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G98" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H98" s="25"/>
+      <c r="I98" s="25"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="27"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>67</v>
@@ -5126,13 +5193,13 @@
         <v>118</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>295</v>
+        <v>210</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>67</v>
@@ -5151,13 +5218,13 @@
         <v>118</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>296</v>
+        <v>211</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>67</v>
@@ -5171,41 +5238,43 @@
       <c r="J101" s="13"/>
       <c r="K101" s="14"/>
     </row>
-    <row r="102" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A102" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B102" s="22"/>
-      <c r="C102" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D102" s="23"/>
-      <c r="E102" s="24" t="s">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="E102" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F102" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G102" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H102" s="25"/>
-      <c r="I102" s="25"/>
-      <c r="J102" s="26"/>
-      <c r="K102" s="27"/>
+      <c r="F102" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="12"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="14"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>208</v>
+        <v>291</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>67</v>
@@ -5221,16 +5290,16 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>213</v>
+        <v>292</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>67</v>
@@ -5244,43 +5313,41 @@
       <c r="J104" s="13"/>
       <c r="K104" s="14"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" s="5" t="s">
+    <row r="105" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A105" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C105" s="5" t="s">
+      <c r="B105" s="22"/>
+      <c r="C105" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="E105" s="4" t="s">
+      <c r="D105" s="23"/>
+      <c r="E105" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F105" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="12"/>
-      <c r="J105" s="13"/>
-      <c r="K105" s="14"/>
+      <c r="F105" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G105" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H105" s="25"/>
+      <c r="I105" s="25"/>
+      <c r="J105" s="26"/>
+      <c r="K105" s="27"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>67</v>
@@ -5294,44 +5361,46 @@
       <c r="J106" s="13"/>
       <c r="K106" s="14"/>
     </row>
-    <row r="107" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A107" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="B107" s="22"/>
-      <c r="C107" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D107" s="23"/>
-      <c r="E107" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F107" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G107" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H107" s="25"/>
-      <c r="I107" s="25"/>
-      <c r="J107" s="26"/>
-      <c r="K107" s="27"/>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="12"/>
+      <c r="J107" s="13"/>
+      <c r="K107" s="14"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>83</v>
@@ -5344,19 +5413,19 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="F109" s="12" t="s">
         <v>83</v>
@@ -5367,43 +5436,41 @@
       <c r="J109" s="13"/>
       <c r="K109" s="14"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A110" s="5" t="s">
+    <row r="110" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A110" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C110" s="5" t="s">
+      <c r="B110" s="22"/>
+      <c r="C110" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D110" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="E110" s="4" t="s">
+      <c r="D110" s="23"/>
+      <c r="E110" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="F110" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="12"/>
-      <c r="J110" s="13"/>
-      <c r="K110" s="14"/>
+      <c r="F110" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G110" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H110" s="25"/>
+      <c r="I110" s="25"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="27"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>95</v>
@@ -5417,46 +5484,48 @@
       <c r="J111" s="13"/>
       <c r="K111" s="14"/>
     </row>
-    <row r="112" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A112" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B112" s="22"/>
-      <c r="C112" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D112" s="23"/>
-      <c r="E112" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="F112" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G112" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H112" s="25"/>
-      <c r="I112" s="25"/>
-      <c r="J112" s="26"/>
-      <c r="K112" s="27"/>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F112" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="12"/>
+      <c r="J112" s="13"/>
+      <c r="K112" s="14"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E113" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F113" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F113" s="12" t="s">
         <v>83</v>
       </c>
       <c r="G113" s="13"/>
@@ -5467,21 +5536,21 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F114" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F114" s="12" t="s">
         <v>83</v>
       </c>
       <c r="G114" s="13"/>
@@ -5490,141 +5559,139 @@
       <c r="J114" s="13"/>
       <c r="K114" s="14"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A115" s="5" t="s">
+    <row r="115" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A115" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B115" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C115" s="5" t="s">
+      <c r="B115" s="22"/>
+      <c r="C115" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E115" s="5" t="s">
+      <c r="D115" s="23"/>
+      <c r="E115" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="F115" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G115" s="13"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="12"/>
-      <c r="J115" s="13"/>
-      <c r="K115" s="14"/>
-    </row>
-    <row r="116" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A116" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B116" s="22"/>
-      <c r="C116" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D116" s="23"/>
-      <c r="E116" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F116" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G116" s="26" t="s">
+      <c r="F115" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G115" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H116" s="25"/>
-      <c r="I116" s="25"/>
-      <c r="J116" s="26"/>
-      <c r="K116" s="27"/>
+      <c r="H115" s="25"/>
+      <c r="I115" s="25"/>
+      <c r="J115" s="26"/>
+      <c r="K115" s="27"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F116" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="12"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="14"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F117" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F117" s="15" t="s">
         <v>83</v>
       </c>
       <c r="G117" s="13"/>
       <c r="H117" s="13"/>
       <c r="I117" s="12"/>
       <c r="J117" s="13"/>
-      <c r="K117" s="13"/>
+      <c r="K117" s="14"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F118" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F118" s="15" t="s">
         <v>83</v>
       </c>
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
       <c r="I118" s="12"/>
       <c r="J118" s="13"/>
-      <c r="K118" s="13"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A119" s="5" t="s">
+      <c r="K118" s="14"/>
+    </row>
+    <row r="119" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A119" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="B119" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C119" s="5" t="s">
+      <c r="B119" s="22"/>
+      <c r="C119" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="E119" s="4" t="s">
+      <c r="D119" s="23"/>
+      <c r="E119" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F119" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="12"/>
-      <c r="J119" s="13"/>
-      <c r="K119" s="13"/>
+      <c r="F119" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G119" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H119" s="25"/>
+      <c r="I119" s="25"/>
+      <c r="J119" s="26"/>
+      <c r="K119" s="27"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>97</v>
@@ -5638,44 +5705,46 @@
       <c r="J120" s="13"/>
       <c r="K120" s="13"/>
     </row>
-    <row r="121" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A121" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B121" s="22"/>
-      <c r="C121" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D121" s="23"/>
-      <c r="E121" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F121" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G121" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H121" s="25"/>
-      <c r="I121" s="25"/>
-      <c r="J121" s="26"/>
-      <c r="K121" s="27"/>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F121" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="12"/>
+      <c r="J121" s="13"/>
+      <c r="K121" s="13"/>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D122" s="5" t="s">
-        <v>356</v>
+        <v>49</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>353</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="F122" s="12" t="s">
         <v>83</v>
@@ -5688,19 +5757,19 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>357</v>
+        <v>49</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="F123" s="12" t="s">
         <v>83</v>
@@ -5709,71 +5778,71 @@
       <c r="H123" s="13"/>
       <c r="I123" s="12"/>
       <c r="J123" s="13"/>
-      <c r="K123" s="16"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A124" s="5" t="s">
+      <c r="K123" s="13"/>
+    </row>
+    <row r="124" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A124" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B124" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C124" s="5" t="s">
+      <c r="B124" s="22"/>
+      <c r="C124" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D124" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E124" s="4" t="s">
+      <c r="D124" s="23"/>
+      <c r="E124" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F124" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="12"/>
-      <c r="J124" s="13"/>
-      <c r="K124" s="16"/>
-    </row>
-    <row r="125" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A125" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B125" s="22"/>
-      <c r="C125" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D125" s="23"/>
-      <c r="E125" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F125" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G125" s="26" t="s">
+      <c r="F124" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G124" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H125" s="25"/>
-      <c r="I125" s="25"/>
-      <c r="J125" s="26"/>
-      <c r="K125" s="27"/>
+      <c r="H124" s="25"/>
+      <c r="I124" s="25"/>
+      <c r="J124" s="26"/>
+      <c r="K124" s="27"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F125" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+      <c r="I125" s="12"/>
+      <c r="J125" s="13"/>
+      <c r="K125" s="13"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>373</v>
+        <v>61</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="F126" s="12" t="s">
         <v>83</v>
@@ -5786,19 +5855,19 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>167</v>
+        <v>220</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>374</v>
+        <v>61</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>350</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="F127" s="12" t="s">
         <v>83</v>
@@ -5809,43 +5878,41 @@
       <c r="J127" s="13"/>
       <c r="K127" s="16"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A128" s="5" t="s">
+    <row r="128" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A128" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B128" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C128" s="5" t="s">
+      <c r="B128" s="22"/>
+      <c r="C128" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="E128" s="4" t="s">
+      <c r="D128" s="23"/>
+      <c r="E128" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F128" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="12"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="16"/>
+      <c r="F128" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G128" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H128" s="25"/>
+      <c r="I128" s="25"/>
+      <c r="J128" s="26"/>
+      <c r="K128" s="27"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>109</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>66</v>
@@ -5864,13 +5931,13 @@
         <v>109</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>66</v>
@@ -5889,13 +5956,13 @@
         <v>109</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>66</v>
@@ -5909,44 +5976,46 @@
       <c r="J131" s="13"/>
       <c r="K131" s="16"/>
     </row>
-    <row r="132" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A132" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="B132" s="22"/>
-      <c r="C132" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D132" s="23"/>
-      <c r="E132" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F132" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G132" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H132" s="25"/>
-      <c r="I132" s="25"/>
-      <c r="J132" s="26"/>
-      <c r="K132" s="27"/>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F132" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="12"/>
+      <c r="J132" s="13"/>
+      <c r="K132" s="16"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>331</v>
+        <v>369</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="F133" s="12" t="s">
         <v>83</v>
@@ -5955,23 +6024,23 @@
       <c r="H133" s="13"/>
       <c r="I133" s="12"/>
       <c r="J133" s="13"/>
-      <c r="K133" s="13"/>
+      <c r="K133" s="16"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>332</v>
+        <v>370</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="F134" s="12" t="s">
         <v>83</v>
@@ -5980,45 +6049,43 @@
       <c r="H134" s="13"/>
       <c r="I134" s="12"/>
       <c r="J134" s="13"/>
-      <c r="K134" s="13"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A135" s="5" t="s">
+      <c r="K134" s="16"/>
+    </row>
+    <row r="135" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A135" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B135" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C135" s="5" t="s">
+      <c r="B135" s="22"/>
+      <c r="C135" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D135" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E135" s="4" t="s">
+      <c r="D135" s="23"/>
+      <c r="E135" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F135" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G135" s="13"/>
-      <c r="H135" s="13"/>
-      <c r="I135" s="12"/>
-      <c r="J135" s="13"/>
-      <c r="K135" s="13"/>
+      <c r="F135" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G135" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H135" s="25"/>
+      <c r="I135" s="25"/>
+      <c r="J135" s="26"/>
+      <c r="K135" s="27"/>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>226</v>
+        <v>164</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>97</v>
@@ -6032,44 +6099,46 @@
       <c r="J136" s="13"/>
       <c r="K136" s="13"/>
     </row>
-    <row r="137" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A137" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B137" s="22"/>
-      <c r="C137" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D137" s="23"/>
-      <c r="E137" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F137" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G137" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H137" s="25"/>
-      <c r="I137" s="25"/>
-      <c r="J137" s="26"/>
-      <c r="K137" s="27"/>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F137" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="12"/>
+      <c r="J137" s="13"/>
+      <c r="K137" s="13"/>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="E138" s="6" t="s">
-        <v>85</v>
+        <v>327</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F138" s="12" t="s">
         <v>83</v>
@@ -6082,19 +6151,19 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="E139" s="6" t="s">
-        <v>85</v>
+        <v>328</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F139" s="12" t="s">
         <v>83</v>
@@ -6105,69 +6174,69 @@
       <c r="J139" s="13"/>
       <c r="K139" s="13"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A140" s="5" t="s">
+    <row r="140" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A140" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B140" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C140" s="5" t="s">
+      <c r="B140" s="22"/>
+      <c r="C140" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D140" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="E140" s="6" t="s">
+      <c r="D140" s="23"/>
+      <c r="E140" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F140" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="12"/>
-      <c r="J140" s="13"/>
-      <c r="K140" s="13"/>
-    </row>
-    <row r="141" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A141" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B141" s="22"/>
-      <c r="C141" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D141" s="23"/>
-      <c r="E141" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F141" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G141" s="26" t="s">
+      <c r="F140" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G140" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H141" s="25"/>
-      <c r="I141" s="25"/>
-      <c r="J141" s="26"/>
-      <c r="K141" s="27"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="25"/>
+      <c r="J140" s="26"/>
+      <c r="K140" s="27"/>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F141" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="12"/>
+      <c r="J141" s="13"/>
+      <c r="K141" s="13"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="E142" s="7" t="s">
-        <v>99</v>
+        <v>330</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="F142" s="12" t="s">
         <v>83</v>
@@ -6180,19 +6249,19 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D143" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="E143" s="7" t="s">
-        <v>99</v>
+        <v>54</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="F143" s="12" t="s">
         <v>83</v>
@@ -6203,43 +6272,41 @@
       <c r="J143" s="13"/>
       <c r="K143" s="13"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A144" s="5" t="s">
+    <row r="144" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A144" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B144" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C144" s="5" t="s">
+      <c r="B144" s="22"/>
+      <c r="C144" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D144" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="E144" s="7" t="s">
+      <c r="D144" s="23"/>
+      <c r="E144" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="F144" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G144" s="13"/>
-      <c r="H144" s="13"/>
-      <c r="I144" s="12"/>
-      <c r="J144" s="13"/>
-      <c r="K144" s="13"/>
+      <c r="F144" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G144" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H144" s="25"/>
+      <c r="I144" s="25"/>
+      <c r="J144" s="26"/>
+      <c r="K144" s="27"/>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D145" s="8" t="s">
-        <v>341</v>
+      <c r="D145" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>99</v>
@@ -6253,44 +6320,46 @@
       <c r="J145" s="13"/>
       <c r="K145" s="13"/>
     </row>
-    <row r="146" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A146" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B146" s="22"/>
-      <c r="C146" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D146" s="23"/>
-      <c r="E146" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F146" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G146" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H146" s="25"/>
-      <c r="I146" s="25"/>
-      <c r="J146" s="26"/>
-      <c r="K146" s="27"/>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F146" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="12"/>
+      <c r="J146" s="13"/>
+      <c r="K146" s="13"/>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>141</v>
+        <v>230</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="E147" s="4" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F147" s="12" t="s">
         <v>83</v>
@@ -6299,23 +6368,23 @@
       <c r="H147" s="13"/>
       <c r="I147" s="12"/>
       <c r="J147" s="13"/>
-      <c r="K147" s="14"/>
+      <c r="K147" s="13"/>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="E148" s="4" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F148" s="12" t="s">
         <v>83</v>
@@ -6324,57 +6393,228 @@
       <c r="H148" s="13"/>
       <c r="I148" s="12"/>
       <c r="J148" s="13"/>
-      <c r="K148" s="14"/>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A149" s="5" t="s">
+      <c r="K148" s="13"/>
+    </row>
+    <row r="149" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A149" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B149" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C149" s="5" t="s">
+      <c r="B149" s="22"/>
+      <c r="C149" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D149" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="E149" s="4" t="s">
+      <c r="D149" s="23"/>
+      <c r="E149" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="F149" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G149" s="13"/>
-      <c r="H149" s="13"/>
-      <c r="I149" s="12"/>
-      <c r="J149" s="13"/>
-      <c r="K149" s="14"/>
+      <c r="F149" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G149" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H149" s="25"/>
+      <c r="I149" s="25"/>
+      <c r="J149" s="26"/>
+      <c r="K149" s="27"/>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A150" s="9" t="s">
+      <c r="A150" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B150" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C150" s="9" t="s">
+      <c r="B150" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C150" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D150" s="10" t="s">
-        <v>345</v>
+      <c r="D150" s="3" t="s">
+        <v>336</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F150" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G150" s="21"/>
-      <c r="H150" s="21"/>
-      <c r="I150" s="20"/>
-      <c r="J150" s="21"/>
+      <c r="F150" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="12"/>
+      <c r="J150" s="13"/>
       <c r="K150" s="14"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F151" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="12"/>
+      <c r="J151" s="13"/>
+      <c r="K151" s="14"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F152" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="12"/>
+      <c r="J152" s="13"/>
+      <c r="K152" s="14"/>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D153" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F153" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G153" s="21"/>
+      <c r="H153" s="21"/>
+      <c r="I153" s="20"/>
+      <c r="J153" s="21"/>
+      <c r="K153" s="14"/>
+    </row>
+    <row r="154" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A154" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="B154" s="22"/>
+      <c r="C154" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="D154" s="23"/>
+      <c r="E154" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F154" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G154" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H154" s="25"/>
+      <c r="I154" s="25"/>
+      <c r="J154" s="26"/>
+      <c r="K154" s="27"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B155" s="49" t="s">
+        <v>373</v>
+      </c>
+      <c r="C155" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="D155" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F155" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G155" s="52"/>
+      <c r="H155" s="52"/>
+      <c r="I155" s="51"/>
+      <c r="J155" s="52"/>
+      <c r="K155" s="53"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B156" s="49" t="s">
+        <v>374</v>
+      </c>
+      <c r="C156" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="D156" s="50" t="s">
+        <v>377</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F156" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G156" s="52"/>
+      <c r="H156" s="52"/>
+      <c r="I156" s="51"/>
+      <c r="J156" s="52"/>
+      <c r="K156" s="53"/>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B157" s="49" t="s">
+        <v>375</v>
+      </c>
+      <c r="C157" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="D157" s="50" t="s">
+        <v>378</v>
+      </c>
+      <c r="E157" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F157" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G157" s="52"/>
+      <c r="H157" s="52"/>
+      <c r="I157" s="51"/>
+      <c r="J157" s="52"/>
+      <c r="K157" s="53"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -6394,19 +6634,19 @@
           <x14:formula1>
             <xm:f>DropDownOptions!$B$7:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G150</xm:sqref>
+          <xm:sqref>G3:G157</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{373109B0-DE85-C548-A398-F123A2DF93DC}">
           <x14:formula1>
             <xm:f>DropDownOptions!$B$8:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F150</xm:sqref>
+          <xm:sqref>F3:F157</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28F579DA-03FB-B444-A7F7-79D1AAF79220}">
           <x14:formula1>
             <xm:f>DropDownOptions!$B$1:$G$1</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I150</xm:sqref>
+          <xm:sqref>I3:I157</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
feat: cf tracker updates (#42)
</commit_message>
<xml_diff>
--- a/trackers-and-planning/cloud-foundations-tracker/Cloud Foundations Tracker.xlsx
+++ b/trackers-and-planning/cloud-foundations-tracker/Cloud Foundations Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awstodd/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awstodd/unCode/Gits/GITHUB-CloudFoundations/cloud-foundations-templates/trackers-and-planning/cloud-foundations-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81B5C18F-8243-6940-92F1-AEB354876859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B1A540-EC60-8C48-920B-FA158FA00823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52500" yWindow="500" windowWidth="49060" windowHeight="23340" xr2:uid="{8357623D-2B7C-8445-9F5B-200FB7F3C4BA}"/>
+    <workbookView xWindow="52500" yWindow="500" windowWidth="49060" windowHeight="23340" activeTab="1" xr2:uid="{8357623D-2B7C-8445-9F5B-200FB7F3C4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="396">
   <si>
     <t>Customer Name</t>
   </si>
@@ -809,24 +809,12 @@
     <t>Patch rollback and recovery</t>
   </si>
   <si>
-    <t>Assess and identify vulnerabilities</t>
-  </si>
-  <si>
-    <t>Respond to vulnerabilities</t>
-  </si>
-  <si>
-    <t>Report on vulnerabilties</t>
-  </si>
-  <si>
     <t>CF7-S5</t>
   </si>
   <si>
     <t>CF8-S5</t>
   </si>
   <si>
-    <t>Design isolated resource environments</t>
-  </si>
-  <si>
     <t>Isolated environment lifecycle management</t>
   </si>
   <si>
@@ -944,12 +932,6 @@
     <t>Evidence reporting</t>
   </si>
   <si>
-    <t>Classify and prioritize vulnerabilities</t>
-  </si>
-  <si>
-    <t>Improve process</t>
-  </si>
-  <si>
     <t>Repeatable patterns for isolated enviornments</t>
   </si>
   <si>
@@ -1070,18 +1052,12 @@
     <t>Change Management Fulfillment</t>
   </si>
   <si>
-    <t>Change Rollback</t>
-  </si>
-  <si>
     <t>Change Monitoring and Assessment</t>
   </si>
   <si>
     <t>Stakeholders</t>
   </si>
   <si>
-    <t>Coming Soon</t>
-  </si>
-  <si>
     <t>Backup requirements and strategy</t>
   </si>
   <si>
@@ -1173,6 +1149,81 @@
   </si>
   <si>
     <t>Compliance management</t>
+  </si>
+  <si>
+    <t>CF31</t>
+  </si>
+  <si>
+    <t>Image Management</t>
+  </si>
+  <si>
+    <t>CF31-S1</t>
+  </si>
+  <si>
+    <t>CF31-S2</t>
+  </si>
+  <si>
+    <t>CF31-S3</t>
+  </si>
+  <si>
+    <t>Image development</t>
+  </si>
+  <si>
+    <t>Image storage and distribution</t>
+  </si>
+  <si>
+    <t>Image lifecycle management</t>
+  </si>
+  <si>
+    <t>Change Rollout/Rollback</t>
+  </si>
+  <si>
+    <t>Support requirements and strategy</t>
+  </si>
+  <si>
+    <t>Ticketing system(s) and integration</t>
+  </si>
+  <si>
+    <t>Support and operational readiness</t>
+  </si>
+  <si>
+    <t>Health monitoring</t>
+  </si>
+  <si>
+    <t>CF12-S5</t>
+  </si>
+  <si>
+    <t>CF12-S6</t>
+  </si>
+  <si>
+    <t>Operational event management</t>
+  </si>
+  <si>
+    <t>Environment access for support</t>
+  </si>
+  <si>
+    <t>CF10-S5</t>
+  </si>
+  <si>
+    <t>Data residency</t>
+  </si>
+  <si>
+    <t>Designing isolated resource environments</t>
+  </si>
+  <si>
+    <t>Process improvement</t>
+  </si>
+  <si>
+    <t>Vulnerability identification and assessment</t>
+  </si>
+  <si>
+    <t>Vulnerability classification and prioritization</t>
+  </si>
+  <si>
+    <t>Vulnerability response</t>
+  </si>
+  <si>
+    <t>Vulnerability reporting</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1586,13 +1637,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -1602,162 +1646,53 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF010022"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF010022"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF010022"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF010022"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF010022"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF010022"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF010022"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF010022"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2089,11 +2024,143 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF010022"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF010022"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF010022"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF010022"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF010022"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF010022"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF010022"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF010022"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF010022"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2180,32 +2247,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C32B6F1C-594B-EF46-9E98-D6C31AE3F5ED}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C32B6F1C-594B-EF46-9E98-D6C31AE3F5ED}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:C8" xr:uid="{458A2142-5A50-7D4E-8042-7BD4B32DCDCE}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3C316A9B-7332-4349-AAA4-7238D66CC0CA}" name="Question" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{7C60BFEC-A699-8843-9E5F-DBE547E55959}" name="Answer" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{329AD68F-C5D6-9A4D-AF8C-830676506BC8}" name="Instructions" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3C316A9B-7332-4349-AAA4-7238D66CC0CA}" name="Question" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7C60BFEC-A699-8843-9E5F-DBE547E55959}" name="Answer" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{329AD68F-C5D6-9A4D-AF8C-830676506BC8}" name="Instructions" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}" name="Table2" displayName="Table2" ref="A2:K150" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A2:K150" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}" name="Table2" displayName="Table2" ref="A2:K157" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K157" xr:uid="{F3413BCC-E94F-A54C-9114-2693FEDA6CFA}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FE1167A3-DF76-D74B-B521-E68F0EB60494}" name="CAP ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{6407AEF3-7924-094D-8A5A-40B9D718CCE6}" name="Scenario ID" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{A748EA53-7C5A-7B4D-87B7-4CB9B473475D}" name="Capability" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{55B54472-AD4E-8445-B71E-3AE1E9AC463C}" name="Scenario" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{573429BF-70FF-C746-8240-F6FD8088D7C8}" name="Stakeholders" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{BF4B01D1-8572-4143-B02F-99490778142C}" name="Completed" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{FDBC1E55-1B33-C64A-A2C1-6432DD8F973F}" name="Stage" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{B1CF695B-93BA-EF4B-BD07-B17D64F157F9}" name="Notes" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{8EAD3560-DBF5-1941-BA7D-9D7E3F958354}" name="Owner" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{F0BC2494-A3E4-8443-A2EF-E1DCC2C91ABE}" name="Feedback" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{EECFCACA-6655-204B-9A4E-DB5D71ED9602}" name="Time to completion (in weeks)" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{FE1167A3-DF76-D74B-B521-E68F0EB60494}" name="CAP ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6407AEF3-7924-094D-8A5A-40B9D718CCE6}" name="Scenario ID" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{A748EA53-7C5A-7B4D-87B7-4CB9B473475D}" name="Capability" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{55B54472-AD4E-8445-B71E-3AE1E9AC463C}" name="Scenario" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{573429BF-70FF-C746-8240-F6FD8088D7C8}" name="Stakeholders" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BF4B01D1-8572-4143-B02F-99490778142C}" name="Completed" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FDBC1E55-1B33-C64A-A2C1-6432DD8F973F}" name="Stage" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{B1CF695B-93BA-EF4B-BD07-B17D64F157F9}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{8EAD3560-DBF5-1941-BA7D-9D7E3F958354}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{F0BC2494-A3E4-8443-A2EF-E1DCC2C91ABE}" name="Feedback" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{EECFCACA-6655-204B-9A4E-DB5D71ED9602}" name="Time to completion (in weeks)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2510,7 +2577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A01F414-5472-0445-9FF4-8BCF3433CDD1}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="224" workbookViewId="0">
+    <sheetView zoomScale="224" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2522,76 +2589,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="45" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="44" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44" t="s">
-        <v>372</v>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2599,8 +2666,8 @@
       <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="2">
-        <f>COUNTIF(Capabilities!$F$3:$F$150,"Yes")</f>
+      <c r="B11" s="54">
+        <f>COUNTIF(Capabilities!$F$3:$F$157,"Yes")</f>
         <v>0</v>
       </c>
     </row>
@@ -2656,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0651646F-D6FF-204E-8928-F8B104176F10}">
-  <dimension ref="A1:K150"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2677,21 +2744,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
-        <v>369</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39" t="s">
-        <v>370</v>
-      </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
+      <c r="A1" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48" t="s">
+        <v>362</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -2707,7 +2774,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>64</v>
@@ -2789,7 +2856,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>84</v>
@@ -2815,7 +2882,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>84</v>
@@ -2889,7 +2956,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>67</v>
@@ -2914,7 +2981,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>67</v>
@@ -2933,13 +3000,13 @@
         <v>120</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>67</v>
@@ -3012,7 +3079,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>67</v>
@@ -3160,7 +3227,7 @@
         <v>56</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>67</v>
@@ -3210,7 +3277,7 @@
         <v>56</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>67</v>
@@ -3230,7 +3297,7 @@
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="24" t="s">
@@ -3255,7 +3322,7 @@
         <v>146</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>252</v>
@@ -3280,7 +3347,7 @@
         <v>156</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>253</v>
@@ -3305,7 +3372,7 @@
         <v>157</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>254</v>
@@ -3330,7 +3397,7 @@
         <v>158</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>255</v>
@@ -3355,7 +3422,7 @@
         <v>159</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>256</v>
@@ -3406,7 +3473,7 @@
         <v>60</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>257</v>
+        <v>392</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>67</v>
@@ -3431,7 +3498,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>302</v>
+        <v>393</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>67</v>
@@ -3456,7 +3523,7 @@
         <v>60</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>258</v>
+        <v>394</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>67</v>
@@ -3481,7 +3548,7 @@
         <v>60</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>259</v>
+        <v>395</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>67</v>
@@ -3506,7 +3573,7 @@
         <v>60</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>303</v>
+        <v>391</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>67</v>
@@ -3548,13 +3615,13 @@
         <v>125</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>262</v>
+        <v>390</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>86</v>
@@ -3573,13 +3640,13 @@
         <v>125</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>86</v>
@@ -3598,13 +3665,13 @@
         <v>125</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>86</v>
@@ -3623,13 +3690,13 @@
         <v>125</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>86</v>
@@ -3677,7 +3744,7 @@
         <v>57</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>87</v>
@@ -3702,7 +3769,7 @@
         <v>57</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>87</v>
@@ -3727,7 +3794,7 @@
         <v>57</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>87</v>
@@ -3752,7 +3819,7 @@
         <v>57</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>87</v>
@@ -3771,13 +3838,13 @@
         <v>126</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>87</v>
@@ -3825,7 +3892,7 @@
         <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>88</v>
@@ -3850,7 +3917,7 @@
         <v>46</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>88</v>
@@ -3875,7 +3942,7 @@
         <v>46</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>88</v>
@@ -3900,7 +3967,7 @@
         <v>46</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>88</v>
@@ -3948,7 +4015,7 @@
         <v>44</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>88</v>
@@ -3973,7 +4040,7 @@
         <v>44</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>88</v>
@@ -3998,7 +4065,7 @@
         <v>44</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>88</v>
@@ -4023,7 +4090,7 @@
         <v>44</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>88</v>
@@ -4037,66 +4104,66 @@
       <c r="J55" s="13"/>
       <c r="K55" s="14"/>
     </row>
-    <row r="56" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="53"/>
+    </row>
+    <row r="57" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22" t="s">
+      <c r="B57" s="22"/>
+      <c r="C57" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="24" t="s">
+      <c r="D57" s="23"/>
+      <c r="E57" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="F56" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G56" s="26" t="s">
+      <c r="F57" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G57" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="27"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="14"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="27"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>89</v>
@@ -4115,13 +4182,13 @@
         <v>111</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>89</v>
@@ -4140,13 +4207,13 @@
         <v>111</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>89</v>
@@ -4165,13 +4232,13 @@
         <v>111</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>285</v>
+        <v>188</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>89</v>
@@ -4190,15 +4257,15 @@
         <v>111</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E62" s="7" t="s">
+      <c r="D62" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F62" s="12" t="s">
@@ -4210,66 +4277,66 @@
       <c r="J62" s="13"/>
       <c r="K62" s="14"/>
     </row>
-    <row r="63" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="14"/>
+    </row>
+    <row r="64" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22" t="s">
+      <c r="B64" s="22"/>
+      <c r="C64" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D63" s="23"/>
-      <c r="E63" s="24" t="s">
+      <c r="D64" s="23"/>
+      <c r="E64" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F63" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G63" s="26" t="s">
+      <c r="F64" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G64" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H63" s="25"/>
-      <c r="I63" s="25"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="27"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F64" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="14"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="27"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>90</v>
@@ -4288,13 +4355,13 @@
         <v>112</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>90</v>
@@ -4313,13 +4380,13 @@
         <v>112</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>90</v>
@@ -4333,147 +4400,149 @@
       <c r="J67" s="13"/>
       <c r="K67" s="14"/>
     </row>
-    <row r="68" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="22" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="14"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="49" t="s">
+        <v>386</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G69" s="52"/>
+      <c r="H69" s="52"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="53"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="49" t="s">
+        <v>385</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="49" t="s">
+        <v>387</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G70" s="52"/>
+      <c r="H70" s="52"/>
+      <c r="I70" s="51"/>
+      <c r="J70" s="52"/>
+      <c r="K70" s="53"/>
+    </row>
+    <row r="71" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22" t="s">
+      <c r="B71" s="22"/>
+      <c r="C71" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="23"/>
-      <c r="E68" s="24" t="s">
+      <c r="D71" s="23"/>
+      <c r="E71" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="F68" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G68" s="26" t="s">
+      <c r="F71" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H68" s="25"/>
-      <c r="I68" s="25"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="27"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="H71" s="25"/>
+      <c r="I71" s="25"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="27"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B72" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="E69" s="6" t="s">
+      <c r="D72" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F69" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F70" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F71" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-    </row>
-    <row r="72" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="D72" s="23"/>
-      <c r="E72" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F72" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G72" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H72" s="25"/>
-      <c r="I72" s="25"/>
-      <c r="J72" s="26"/>
-      <c r="K72" s="27"/>
+      <c r="F72" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G73" s="19"/>
+        <v>301</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F73" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G73" s="13"/>
       <c r="H73" s="13"/>
       <c r="I73" s="12"/>
       <c r="J73" s="13"/>
@@ -4481,66 +4550,64 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F74" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G74" s="19"/>
+        <v>284</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G74" s="13"/>
       <c r="H74" s="13"/>
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
-      <c r="K74" s="16"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
+      <c r="K74" s="13"/>
+    </row>
+    <row r="75" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="E75" s="4" t="s">
+      <c r="B75" s="22"/>
+      <c r="C75" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="F75" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G75" s="19"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="16"/>
+      <c r="F75" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G75" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H75" s="25"/>
+      <c r="I75" s="25"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="27"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>91</v>
@@ -4552,20 +4619,20 @@
       <c r="H76" s="13"/>
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
-      <c r="K76" s="16"/>
+      <c r="K76" s="13"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>240</v>
+        <v>194</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>91</v>
@@ -4584,13 +4651,13 @@
         <v>106</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>368</v>
+        <v>304</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>91</v>
@@ -4604,44 +4671,46 @@
       <c r="J78" s="13"/>
       <c r="K78" s="16"/>
     </row>
-    <row r="79" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A79" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B79" s="22"/>
-      <c r="C79" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D79" s="23"/>
-      <c r="E79" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F79" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G79" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H79" s="25"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="26"/>
-      <c r="K79" s="27"/>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G79" s="19"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="16"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>182</v>
+        <v>240</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>107</v>
+        <v>359</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>83</v>
@@ -4654,19 +4723,19 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>107</v>
+        <v>359</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>313</v>
+        <v>360</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F81" s="18" t="s">
         <v>83</v>
@@ -4677,43 +4746,41 @@
       <c r="J81" s="13"/>
       <c r="K81" s="16"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+    <row r="82" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C82" s="5" t="s">
+      <c r="B82" s="22"/>
+      <c r="C82" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D82" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E82" s="4" t="s">
+      <c r="D82" s="23"/>
+      <c r="E82" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="F82" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G82" s="19"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="16"/>
+      <c r="F82" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G82" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H82" s="25"/>
+      <c r="I82" s="25"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="27"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>107</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>92</v>
@@ -4732,13 +4799,13 @@
         <v>108</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>107</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>92</v>
@@ -4752,116 +4819,116 @@
       <c r="J84" s="13"/>
       <c r="K84" s="16"/>
     </row>
-    <row r="85" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B85" s="22"/>
-      <c r="C85" s="22" t="s">
-        <v>317</v>
-      </c>
-      <c r="D85" s="23"/>
-      <c r="E85" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F85" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G85" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H85" s="25"/>
-      <c r="I85" s="25"/>
-      <c r="J85" s="26"/>
-      <c r="K85" s="27"/>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G85" s="19"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="16"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>317</v>
+        <v>107</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F86" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G86" s="13"/>
+        <v>92</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G86" s="19"/>
       <c r="H86" s="13"/>
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
+      <c r="K86" s="16"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>317</v>
+        <v>107</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>349</v>
+        <v>310</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F87" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G87" s="13"/>
+        <v>92</v>
+      </c>
+      <c r="F87" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G87" s="19"/>
       <c r="H87" s="13"/>
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
+      <c r="K87" s="16"/>
+    </row>
+    <row r="88" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="E88" s="4" t="s">
+      <c r="B88" s="22"/>
+      <c r="C88" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="D88" s="23"/>
+      <c r="E88" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="F88" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
+      <c r="F88" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G88" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="27"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>94</v>
@@ -4880,13 +4947,13 @@
         <v>113</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>290</v>
+        <v>202</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>94</v>
@@ -4900,44 +4967,46 @@
       <c r="J90" s="13"/>
       <c r="K90" s="13"/>
     </row>
-    <row r="91" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A91" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B91" s="22"/>
-      <c r="C91" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" s="23"/>
-      <c r="E91" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F91" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G91" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H91" s="25"/>
-      <c r="I91" s="25"/>
-      <c r="J91" s="26"/>
-      <c r="K91" s="27"/>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F91" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="13"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>50</v>
+        <v>311</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F92" s="12" t="s">
         <v>83</v>
@@ -4950,19 +5019,19 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>205</v>
+        <v>286</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>50</v>
+        <v>311</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F93" s="12" t="s">
         <v>83</v>
@@ -4973,69 +5042,69 @@
       <c r="J93" s="13"/>
       <c r="K93" s="13"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+    <row r="94" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="B94" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C94" s="5" t="s">
+      <c r="B94" s="22"/>
+      <c r="C94" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D94" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="E94" s="4" t="s">
+      <c r="D94" s="23"/>
+      <c r="E94" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="F94" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="12"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-    </row>
-    <row r="95" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A95" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B95" s="22"/>
-      <c r="C95" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D95" s="23"/>
-      <c r="E95" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F95" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G95" s="26" t="s">
+      <c r="F94" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G94" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H95" s="25"/>
-      <c r="I95" s="25"/>
-      <c r="J95" s="26"/>
-      <c r="K95" s="27"/>
+      <c r="H94" s="25"/>
+      <c r="I94" s="25"/>
+      <c r="J94" s="26"/>
+      <c r="K94" s="27"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="13"/>
+      <c r="K95" s="13"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>83</v>
@@ -5044,23 +5113,23 @@
       <c r="H96" s="13"/>
       <c r="I96" s="12"/>
       <c r="J96" s="13"/>
-      <c r="K96" s="14"/>
+      <c r="K96" s="13"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>291</v>
+        <v>347</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>83</v>
@@ -5069,45 +5138,43 @@
       <c r="H97" s="13"/>
       <c r="I97" s="12"/>
       <c r="J97" s="13"/>
-      <c r="K97" s="14"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
+      <c r="K97" s="13"/>
+    </row>
+    <row r="98" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C98" s="5" t="s">
+      <c r="B98" s="22"/>
+      <c r="C98" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="E98" s="4" t="s">
+      <c r="D98" s="23"/>
+      <c r="E98" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F98" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="12"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="14"/>
+      <c r="F98" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G98" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H98" s="25"/>
+      <c r="I98" s="25"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="27"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>67</v>
@@ -5126,13 +5193,13 @@
         <v>118</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>295</v>
+        <v>210</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>67</v>
@@ -5151,13 +5218,13 @@
         <v>118</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>296</v>
+        <v>211</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>67</v>
@@ -5171,41 +5238,43 @@
       <c r="J101" s="13"/>
       <c r="K101" s="14"/>
     </row>
-    <row r="102" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A102" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B102" s="22"/>
-      <c r="C102" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D102" s="23"/>
-      <c r="E102" s="24" t="s">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="E102" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F102" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G102" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H102" s="25"/>
-      <c r="I102" s="25"/>
-      <c r="J102" s="26"/>
-      <c r="K102" s="27"/>
+      <c r="F102" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="12"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="14"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>208</v>
+        <v>291</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>67</v>
@@ -5221,16 +5290,16 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>213</v>
+        <v>292</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>67</v>
@@ -5244,43 +5313,41 @@
       <c r="J104" s="13"/>
       <c r="K104" s="14"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" s="5" t="s">
+    <row r="105" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A105" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C105" s="5" t="s">
+      <c r="B105" s="22"/>
+      <c r="C105" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="E105" s="4" t="s">
+      <c r="D105" s="23"/>
+      <c r="E105" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F105" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="12"/>
-      <c r="J105" s="13"/>
-      <c r="K105" s="14"/>
+      <c r="F105" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G105" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H105" s="25"/>
+      <c r="I105" s="25"/>
+      <c r="J105" s="26"/>
+      <c r="K105" s="27"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>67</v>
@@ -5294,44 +5361,46 @@
       <c r="J106" s="13"/>
       <c r="K106" s="14"/>
     </row>
-    <row r="107" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A107" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="B107" s="22"/>
-      <c r="C107" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D107" s="23"/>
-      <c r="E107" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F107" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G107" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H107" s="25"/>
-      <c r="I107" s="25"/>
-      <c r="J107" s="26"/>
-      <c r="K107" s="27"/>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="12"/>
+      <c r="J107" s="13"/>
+      <c r="K107" s="14"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>83</v>
@@ -5344,19 +5413,19 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="F109" s="12" t="s">
         <v>83</v>
@@ -5367,43 +5436,41 @@
       <c r="J109" s="13"/>
       <c r="K109" s="14"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A110" s="5" t="s">
+    <row r="110" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A110" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C110" s="5" t="s">
+      <c r="B110" s="22"/>
+      <c r="C110" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D110" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="E110" s="4" t="s">
+      <c r="D110" s="23"/>
+      <c r="E110" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="F110" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="12"/>
-      <c r="J110" s="13"/>
-      <c r="K110" s="14"/>
+      <c r="F110" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G110" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H110" s="25"/>
+      <c r="I110" s="25"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="27"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>95</v>
@@ -5417,46 +5484,48 @@
       <c r="J111" s="13"/>
       <c r="K111" s="14"/>
     </row>
-    <row r="112" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A112" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B112" s="22"/>
-      <c r="C112" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D112" s="23"/>
-      <c r="E112" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="F112" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G112" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H112" s="25"/>
-      <c r="I112" s="25"/>
-      <c r="J112" s="26"/>
-      <c r="K112" s="27"/>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F112" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="12"/>
+      <c r="J112" s="13"/>
+      <c r="K112" s="14"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E113" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F113" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F113" s="12" t="s">
         <v>83</v>
       </c>
       <c r="G113" s="13"/>
@@ -5467,21 +5536,21 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F114" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F114" s="12" t="s">
         <v>83</v>
       </c>
       <c r="G114" s="13"/>
@@ -5490,141 +5559,139 @@
       <c r="J114" s="13"/>
       <c r="K114" s="14"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A115" s="5" t="s">
+    <row r="115" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A115" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B115" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C115" s="5" t="s">
+      <c r="B115" s="22"/>
+      <c r="C115" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E115" s="5" t="s">
+      <c r="D115" s="23"/>
+      <c r="E115" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="F115" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G115" s="13"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="12"/>
-      <c r="J115" s="13"/>
-      <c r="K115" s="14"/>
-    </row>
-    <row r="116" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A116" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B116" s="22"/>
-      <c r="C116" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D116" s="23"/>
-      <c r="E116" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F116" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G116" s="26" t="s">
+      <c r="F115" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G115" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H116" s="25"/>
-      <c r="I116" s="25"/>
-      <c r="J116" s="26"/>
-      <c r="K116" s="27"/>
+      <c r="H115" s="25"/>
+      <c r="I115" s="25"/>
+      <c r="J115" s="26"/>
+      <c r="K115" s="27"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F116" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="12"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="14"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F117" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F117" s="15" t="s">
         <v>83</v>
       </c>
       <c r="G117" s="13"/>
       <c r="H117" s="13"/>
       <c r="I117" s="12"/>
       <c r="J117" s="13"/>
-      <c r="K117" s="13"/>
+      <c r="K117" s="14"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F118" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F118" s="15" t="s">
         <v>83</v>
       </c>
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
       <c r="I118" s="12"/>
       <c r="J118" s="13"/>
-      <c r="K118" s="13"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A119" s="5" t="s">
+      <c r="K118" s="14"/>
+    </row>
+    <row r="119" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A119" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="B119" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C119" s="5" t="s">
+      <c r="B119" s="22"/>
+      <c r="C119" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="E119" s="4" t="s">
+      <c r="D119" s="23"/>
+      <c r="E119" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F119" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="12"/>
-      <c r="J119" s="13"/>
-      <c r="K119" s="13"/>
+      <c r="F119" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G119" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H119" s="25"/>
+      <c r="I119" s="25"/>
+      <c r="J119" s="26"/>
+      <c r="K119" s="27"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>97</v>
@@ -5638,44 +5705,46 @@
       <c r="J120" s="13"/>
       <c r="K120" s="13"/>
     </row>
-    <row r="121" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A121" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B121" s="22"/>
-      <c r="C121" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D121" s="23"/>
-      <c r="E121" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F121" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G121" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H121" s="25"/>
-      <c r="I121" s="25"/>
-      <c r="J121" s="26"/>
-      <c r="K121" s="27"/>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F121" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="12"/>
+      <c r="J121" s="13"/>
+      <c r="K121" s="13"/>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D122" s="5" t="s">
-        <v>356</v>
+        <v>49</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>353</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="F122" s="12" t="s">
         <v>83</v>
@@ -5688,19 +5757,19 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>357</v>
+        <v>49</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="F123" s="12" t="s">
         <v>83</v>
@@ -5709,71 +5778,71 @@
       <c r="H123" s="13"/>
       <c r="I123" s="12"/>
       <c r="J123" s="13"/>
-      <c r="K123" s="16"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A124" s="5" t="s">
+      <c r="K123" s="13"/>
+    </row>
+    <row r="124" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A124" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B124" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C124" s="5" t="s">
+      <c r="B124" s="22"/>
+      <c r="C124" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D124" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="E124" s="4" t="s">
+      <c r="D124" s="23"/>
+      <c r="E124" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F124" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="12"/>
-      <c r="J124" s="13"/>
-      <c r="K124" s="16"/>
-    </row>
-    <row r="125" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A125" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B125" s="22"/>
-      <c r="C125" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D125" s="23"/>
-      <c r="E125" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F125" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G125" s="26" t="s">
+      <c r="F124" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G124" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H125" s="25"/>
-      <c r="I125" s="25"/>
-      <c r="J125" s="26"/>
-      <c r="K125" s="27"/>
+      <c r="H124" s="25"/>
+      <c r="I124" s="25"/>
+      <c r="J124" s="26"/>
+      <c r="K124" s="27"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F125" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+      <c r="I125" s="12"/>
+      <c r="J125" s="13"/>
+      <c r="K125" s="13"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>373</v>
+        <v>61</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="F126" s="12" t="s">
         <v>83</v>
@@ -5786,19 +5855,19 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>167</v>
+        <v>220</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>374</v>
+        <v>61</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>350</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="F127" s="12" t="s">
         <v>83</v>
@@ -5809,43 +5878,41 @@
       <c r="J127" s="13"/>
       <c r="K127" s="16"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A128" s="5" t="s">
+    <row r="128" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A128" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B128" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C128" s="5" t="s">
+      <c r="B128" s="22"/>
+      <c r="C128" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="E128" s="4" t="s">
+      <c r="D128" s="23"/>
+      <c r="E128" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F128" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="12"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="16"/>
+      <c r="F128" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G128" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H128" s="25"/>
+      <c r="I128" s="25"/>
+      <c r="J128" s="26"/>
+      <c r="K128" s="27"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>109</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>66</v>
@@ -5864,13 +5931,13 @@
         <v>109</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>66</v>
@@ -5889,13 +5956,13 @@
         <v>109</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>66</v>
@@ -5909,44 +5976,46 @@
       <c r="J131" s="13"/>
       <c r="K131" s="16"/>
     </row>
-    <row r="132" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A132" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="B132" s="22"/>
-      <c r="C132" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D132" s="23"/>
-      <c r="E132" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F132" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G132" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H132" s="25"/>
-      <c r="I132" s="25"/>
-      <c r="J132" s="26"/>
-      <c r="K132" s="27"/>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F132" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="12"/>
+      <c r="J132" s="13"/>
+      <c r="K132" s="16"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>331</v>
+        <v>369</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="F133" s="12" t="s">
         <v>83</v>
@@ -5955,23 +6024,23 @@
       <c r="H133" s="13"/>
       <c r="I133" s="12"/>
       <c r="J133" s="13"/>
-      <c r="K133" s="13"/>
+      <c r="K133" s="16"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>332</v>
+        <v>370</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="F134" s="12" t="s">
         <v>83</v>
@@ -5980,45 +6049,43 @@
       <c r="H134" s="13"/>
       <c r="I134" s="12"/>
       <c r="J134" s="13"/>
-      <c r="K134" s="13"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A135" s="5" t="s">
+      <c r="K134" s="16"/>
+    </row>
+    <row r="135" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A135" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B135" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C135" s="5" t="s">
+      <c r="B135" s="22"/>
+      <c r="C135" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D135" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E135" s="4" t="s">
+      <c r="D135" s="23"/>
+      <c r="E135" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F135" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G135" s="13"/>
-      <c r="H135" s="13"/>
-      <c r="I135" s="12"/>
-      <c r="J135" s="13"/>
-      <c r="K135" s="13"/>
+      <c r="F135" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G135" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H135" s="25"/>
+      <c r="I135" s="25"/>
+      <c r="J135" s="26"/>
+      <c r="K135" s="27"/>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>226</v>
+        <v>164</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>97</v>
@@ -6032,44 +6099,46 @@
       <c r="J136" s="13"/>
       <c r="K136" s="13"/>
     </row>
-    <row r="137" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A137" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B137" s="22"/>
-      <c r="C137" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D137" s="23"/>
-      <c r="E137" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F137" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G137" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H137" s="25"/>
-      <c r="I137" s="25"/>
-      <c r="J137" s="26"/>
-      <c r="K137" s="27"/>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F137" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="12"/>
+      <c r="J137" s="13"/>
+      <c r="K137" s="13"/>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="E138" s="6" t="s">
-        <v>85</v>
+        <v>327</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F138" s="12" t="s">
         <v>83</v>
@@ -6082,19 +6151,19 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="E139" s="6" t="s">
-        <v>85</v>
+        <v>328</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F139" s="12" t="s">
         <v>83</v>
@@ -6105,69 +6174,69 @@
       <c r="J139" s="13"/>
       <c r="K139" s="13"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A140" s="5" t="s">
+    <row r="140" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A140" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B140" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C140" s="5" t="s">
+      <c r="B140" s="22"/>
+      <c r="C140" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D140" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="E140" s="6" t="s">
+      <c r="D140" s="23"/>
+      <c r="E140" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F140" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="12"/>
-      <c r="J140" s="13"/>
-      <c r="K140" s="13"/>
-    </row>
-    <row r="141" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A141" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B141" s="22"/>
-      <c r="C141" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D141" s="23"/>
-      <c r="E141" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F141" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G141" s="26" t="s">
+      <c r="F140" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G140" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H141" s="25"/>
-      <c r="I141" s="25"/>
-      <c r="J141" s="26"/>
-      <c r="K141" s="27"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="25"/>
+      <c r="J140" s="26"/>
+      <c r="K140" s="27"/>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F141" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="12"/>
+      <c r="J141" s="13"/>
+      <c r="K141" s="13"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="E142" s="7" t="s">
-        <v>99</v>
+        <v>330</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="F142" s="12" t="s">
         <v>83</v>
@@ -6180,19 +6249,19 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D143" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="E143" s="7" t="s">
-        <v>99</v>
+        <v>54</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="F143" s="12" t="s">
         <v>83</v>
@@ -6203,43 +6272,41 @@
       <c r="J143" s="13"/>
       <c r="K143" s="13"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A144" s="5" t="s">
+    <row r="144" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A144" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B144" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C144" s="5" t="s">
+      <c r="B144" s="22"/>
+      <c r="C144" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D144" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="E144" s="7" t="s">
+      <c r="D144" s="23"/>
+      <c r="E144" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="F144" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G144" s="13"/>
-      <c r="H144" s="13"/>
-      <c r="I144" s="12"/>
-      <c r="J144" s="13"/>
-      <c r="K144" s="13"/>
+      <c r="F144" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G144" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H144" s="25"/>
+      <c r="I144" s="25"/>
+      <c r="J144" s="26"/>
+      <c r="K144" s="27"/>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D145" s="8" t="s">
-        <v>341</v>
+      <c r="D145" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>99</v>
@@ -6253,44 +6320,46 @@
       <c r="J145" s="13"/>
       <c r="K145" s="13"/>
     </row>
-    <row r="146" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A146" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B146" s="22"/>
-      <c r="C146" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D146" s="23"/>
-      <c r="E146" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F146" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G146" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="H146" s="25"/>
-      <c r="I146" s="25"/>
-      <c r="J146" s="26"/>
-      <c r="K146" s="27"/>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F146" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="12"/>
+      <c r="J146" s="13"/>
+      <c r="K146" s="13"/>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>141</v>
+        <v>230</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="E147" s="4" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F147" s="12" t="s">
         <v>83</v>
@@ -6299,23 +6368,23 @@
       <c r="H147" s="13"/>
       <c r="I147" s="12"/>
       <c r="J147" s="13"/>
-      <c r="K147" s="14"/>
+      <c r="K147" s="13"/>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="E148" s="4" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F148" s="12" t="s">
         <v>83</v>
@@ -6324,57 +6393,228 @@
       <c r="H148" s="13"/>
       <c r="I148" s="12"/>
       <c r="J148" s="13"/>
-      <c r="K148" s="14"/>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A149" s="5" t="s">
+      <c r="K148" s="13"/>
+    </row>
+    <row r="149" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A149" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B149" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C149" s="5" t="s">
+      <c r="B149" s="22"/>
+      <c r="C149" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D149" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="E149" s="4" t="s">
+      <c r="D149" s="23"/>
+      <c r="E149" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="F149" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G149" s="13"/>
-      <c r="H149" s="13"/>
-      <c r="I149" s="12"/>
-      <c r="J149" s="13"/>
-      <c r="K149" s="14"/>
+      <c r="F149" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G149" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H149" s="25"/>
+      <c r="I149" s="25"/>
+      <c r="J149" s="26"/>
+      <c r="K149" s="27"/>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A150" s="9" t="s">
+      <c r="A150" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B150" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C150" s="9" t="s">
+      <c r="B150" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C150" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D150" s="10" t="s">
-        <v>345</v>
+      <c r="D150" s="3" t="s">
+        <v>336</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F150" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G150" s="21"/>
-      <c r="H150" s="21"/>
-      <c r="I150" s="20"/>
-      <c r="J150" s="21"/>
+      <c r="F150" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="12"/>
+      <c r="J150" s="13"/>
       <c r="K150" s="14"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F151" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="12"/>
+      <c r="J151" s="13"/>
+      <c r="K151" s="14"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F152" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="12"/>
+      <c r="J152" s="13"/>
+      <c r="K152" s="14"/>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D153" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F153" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G153" s="21"/>
+      <c r="H153" s="21"/>
+      <c r="I153" s="20"/>
+      <c r="J153" s="21"/>
+      <c r="K153" s="14"/>
+    </row>
+    <row r="154" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A154" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="B154" s="22"/>
+      <c r="C154" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="D154" s="23"/>
+      <c r="E154" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F154" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G154" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H154" s="25"/>
+      <c r="I154" s="25"/>
+      <c r="J154" s="26"/>
+      <c r="K154" s="27"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B155" s="49" t="s">
+        <v>373</v>
+      </c>
+      <c r="C155" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="D155" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F155" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G155" s="52"/>
+      <c r="H155" s="52"/>
+      <c r="I155" s="51"/>
+      <c r="J155" s="52"/>
+      <c r="K155" s="53"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B156" s="49" t="s">
+        <v>374</v>
+      </c>
+      <c r="C156" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="D156" s="50" t="s">
+        <v>377</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F156" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G156" s="52"/>
+      <c r="H156" s="52"/>
+      <c r="I156" s="51"/>
+      <c r="J156" s="52"/>
+      <c r="K156" s="53"/>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B157" s="49" t="s">
+        <v>375</v>
+      </c>
+      <c r="C157" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="D157" s="50" t="s">
+        <v>378</v>
+      </c>
+      <c r="E157" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F157" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G157" s="52"/>
+      <c r="H157" s="52"/>
+      <c r="I157" s="51"/>
+      <c r="J157" s="52"/>
+      <c r="K157" s="53"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -6394,19 +6634,19 @@
           <x14:formula1>
             <xm:f>DropDownOptions!$B$7:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G150</xm:sqref>
+          <xm:sqref>G3:G157</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{373109B0-DE85-C548-A398-F123A2DF93DC}">
           <x14:formula1>
             <xm:f>DropDownOptions!$B$8:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F150</xm:sqref>
+          <xm:sqref>F3:F157</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28F579DA-03FB-B444-A7F7-79D1AAF79220}">
           <x14:formula1>
             <xm:f>DropDownOptions!$B$1:$G$1</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I150</xm:sqref>
+          <xm:sqref>I3:I157</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fix: tracker documentation (#45)
</commit_message>
<xml_diff>
--- a/trackers-and-planning/cloud-foundations-tracker/Cloud Foundations Tracker.xlsx
+++ b/trackers-and-planning/cloud-foundations-tracker/Cloud Foundations Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awstodd/unCode/Gits/GITHUB-CloudFoundations/cloud-foundations-templates/trackers-and-planning/cloud-foundations-tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grolston/github/grolston/cloud-foundations-templates/trackers-and-planning/cloud-foundations-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B1A540-EC60-8C48-920B-FA158FA00823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F323838C-6DDD-8D46-8F51-ED54CF8E8589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52500" yWindow="500" windowWidth="49060" windowHeight="23340" activeTab="1" xr2:uid="{8357623D-2B7C-8445-9F5B-200FB7F3C4BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{8357623D-2B7C-8445-9F5B-200FB7F3C4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -22,20 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="397">
   <si>
     <t>Customer Name</t>
   </si>
@@ -932,9 +924,6 @@
     <t>Evidence reporting</t>
   </si>
   <si>
-    <t>Repeatable patterns for isolated enviornments</t>
-  </si>
-  <si>
     <t>Network intrusion detection</t>
   </si>
   <si>
@@ -1013,9 +1002,6 @@
     <t>Tag usage</t>
   </si>
   <si>
-    <t>Records classfication</t>
-  </si>
-  <si>
     <t>Records lifecycle</t>
   </si>
   <si>
@@ -1224,6 +1210,15 @@
   </si>
   <si>
     <t>Vulnerability reporting</t>
+  </si>
+  <si>
+    <t>CF15-S6</t>
+  </si>
+  <si>
+    <t>Repeatable patterns for isolated environments</t>
+  </si>
+  <si>
+    <t>Records classification</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1664,6 +1659,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1671,22 +1667,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -2641,7 +2621,7 @@
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="42" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2666,7 +2646,7 @@
       <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="47">
         <f>COUNTIF(Capabilities!$F$3:$F$157,"Yes")</f>
         <v>0</v>
       </c>
@@ -2725,8 +2705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0651646F-D6FF-204E-8928-F8B104176F10}">
   <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2744,21 +2724,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
-        <v>362</v>
-      </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="A1" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="49" t="s">
+        <v>360</v>
+      </c>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
     </row>
     <row r="2" spans="1:11" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -2774,7 +2754,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>64</v>
@@ -2956,7 +2936,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>67</v>
@@ -2981,7 +2961,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>67</v>
@@ -3000,13 +2980,13 @@
         <v>120</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>67</v>
@@ -3297,7 +3277,7 @@
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="24" t="s">
@@ -3322,7 +3302,7 @@
         <v>146</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>252</v>
@@ -3347,7 +3327,7 @@
         <v>156</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>253</v>
@@ -3372,7 +3352,7 @@
         <v>157</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>254</v>
@@ -3397,7 +3377,7 @@
         <v>158</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>255</v>
@@ -3422,7 +3402,7 @@
         <v>159</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>256</v>
@@ -3473,7 +3453,7 @@
         <v>60</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>67</v>
@@ -3498,7 +3478,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>67</v>
@@ -3523,7 +3503,7 @@
         <v>60</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>67</v>
@@ -3548,7 +3528,7 @@
         <v>60</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>67</v>
@@ -3573,7 +3553,7 @@
         <v>60</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>67</v>
@@ -3621,7 +3601,7 @@
         <v>62</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>86</v>
@@ -3696,7 +3676,7 @@
         <v>62</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>298</v>
+        <v>395</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>86</v>
@@ -3794,7 +3774,7 @@
         <v>57</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>87</v>
@@ -3844,7 +3824,7 @@
         <v>57</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>87</v>
@@ -4109,13 +4089,13 @@
         <v>117</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>88</v>
@@ -4123,11 +4103,11 @@
       <c r="F56" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G56" s="52"/>
-      <c r="H56" s="52"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="52"/>
-      <c r="K56" s="53"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="14"/>
     </row>
     <row r="57" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
@@ -4336,7 +4316,7 @@
         <v>42</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>90</v>
@@ -4361,7 +4341,7 @@
         <v>42</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>90</v>
@@ -4386,7 +4366,7 @@
         <v>42</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>90</v>
@@ -4411,7 +4391,7 @@
         <v>42</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>90</v>
@@ -4426,17 +4406,17 @@
       <c r="K68" s="14"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="49" t="s">
+      <c r="A69" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B69" s="49" t="s">
-        <v>384</v>
+      <c r="B69" s="5" t="s">
+        <v>382</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="49" t="s">
-        <v>386</v>
+      <c r="D69" s="5" t="s">
+        <v>384</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>90</v>
@@ -4444,24 +4424,24 @@
       <c r="F69" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G69" s="52"/>
-      <c r="H69" s="52"/>
-      <c r="I69" s="51"/>
-      <c r="J69" s="52"/>
-      <c r="K69" s="53"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="14"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="49" t="s">
-        <v>385</v>
+      <c r="B70" s="5" t="s">
+        <v>383</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D70" s="49" t="s">
-        <v>387</v>
+      <c r="D70" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>90</v>
@@ -4469,11 +4449,11 @@
       <c r="F70" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G70" s="52"/>
-      <c r="H70" s="52"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="52"/>
-      <c r="K70" s="53"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="14"/>
     </row>
     <row r="71" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="s">
@@ -4534,7 +4514,7 @@
         <v>41</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>133</v>
@@ -4579,7 +4559,7 @@
       </c>
       <c r="B75" s="22"/>
       <c r="C75" s="22" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D75" s="23"/>
       <c r="E75" s="24" t="s">
@@ -4604,10 +4584,10 @@
         <v>181</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>91</v>
@@ -4629,10 +4609,10 @@
         <v>194</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>91</v>
@@ -4654,10 +4634,10 @@
         <v>195</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>91</v>
@@ -4679,10 +4659,10 @@
         <v>196</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>91</v>
@@ -4704,7 +4684,7 @@
         <v>240</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>285</v>
@@ -4726,13 +4706,13 @@
         <v>106</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>240</v>
+        <v>394</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>91</v>
@@ -4780,7 +4760,7 @@
         <v>107</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>92</v>
@@ -4805,7 +4785,7 @@
         <v>107</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>92</v>
@@ -4830,7 +4810,7 @@
         <v>107</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>92</v>
@@ -4855,7 +4835,7 @@
         <v>107</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>92</v>
@@ -4880,7 +4860,7 @@
         <v>107</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>92</v>
@@ -4900,7 +4880,7 @@
       </c>
       <c r="B88" s="22"/>
       <c r="C88" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D88" s="23"/>
       <c r="E88" s="24" t="s">
@@ -4925,10 +4905,10 @@
         <v>200</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>94</v>
@@ -4950,10 +4930,10 @@
         <v>202</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>94</v>
@@ -4975,10 +4955,10 @@
         <v>203</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>94</v>
@@ -5000,10 +4980,10 @@
         <v>204</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>94</v>
@@ -5025,10 +5005,10 @@
         <v>286</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>94</v>
@@ -5076,7 +5056,7 @@
         <v>50</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>93</v>
@@ -5101,7 +5081,7 @@
         <v>50</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>93</v>
@@ -5126,7 +5106,7 @@
         <v>50</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>93</v>
@@ -5174,7 +5154,7 @@
         <v>47</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>67</v>
@@ -5224,7 +5204,7 @@
         <v>47</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>67</v>
@@ -5347,7 +5327,7 @@
         <v>48</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>67</v>
@@ -5372,7 +5352,7 @@
         <v>48</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>67</v>
@@ -5397,7 +5377,7 @@
         <v>48</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>67</v>
@@ -5422,7 +5402,7 @@
         <v>48</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>67</v>
@@ -5470,7 +5450,7 @@
         <v>43</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>95</v>
@@ -5495,7 +5475,7 @@
         <v>43</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>95</v>
@@ -5520,7 +5500,7 @@
         <v>43</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>95</v>
@@ -5545,7 +5525,7 @@
         <v>43</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>95</v>
@@ -5593,7 +5573,7 @@
         <v>45</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>96</v>
@@ -5618,7 +5598,7 @@
         <v>45</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>96</v>
@@ -5643,7 +5623,7 @@
         <v>45</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>96</v>
@@ -5691,7 +5671,7 @@
         <v>49</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>97</v>
@@ -5716,7 +5696,7 @@
         <v>49</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>97</v>
@@ -5741,7 +5721,7 @@
         <v>49</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E122" s="4" t="s">
         <v>97</v>
@@ -5766,7 +5746,7 @@
         <v>49</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>97</v>
@@ -5814,7 +5794,7 @@
         <v>61</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>132</v>
@@ -5839,7 +5819,7 @@
         <v>61</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>132</v>
@@ -5864,7 +5844,7 @@
         <v>61</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>132</v>
@@ -5912,7 +5892,7 @@
         <v>58</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>66</v>
@@ -5937,7 +5917,7 @@
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>66</v>
@@ -5962,7 +5942,7 @@
         <v>58</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>66</v>
@@ -5987,7 +5967,7 @@
         <v>58</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E132" s="4" t="s">
         <v>66</v>
@@ -6012,7 +5992,7 @@
         <v>58</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>66</v>
@@ -6037,7 +6017,7 @@
         <v>58</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>66</v>
@@ -6085,7 +6065,7 @@
         <v>52</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>325</v>
+        <v>396</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>97</v>
@@ -6110,7 +6090,7 @@
         <v>52</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>97</v>
@@ -6135,7 +6115,7 @@
         <v>52</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>97</v>
@@ -6160,7 +6140,7 @@
         <v>52</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>97</v>
@@ -6208,7 +6188,7 @@
         <v>54</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E141" s="6" t="s">
         <v>85</v>
@@ -6233,7 +6213,7 @@
         <v>54</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>85</v>
@@ -6258,7 +6238,7 @@
         <v>54</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>85</v>
@@ -6306,7 +6286,7 @@
         <v>55</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>99</v>
@@ -6331,7 +6311,7 @@
         <v>55</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E146" s="7" t="s">
         <v>99</v>
@@ -6356,7 +6336,7 @@
         <v>55</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>99</v>
@@ -6381,7 +6361,7 @@
         <v>55</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E148" s="7" t="s">
         <v>99</v>
@@ -6429,7 +6409,7 @@
         <v>63</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>98</v>
@@ -6454,7 +6434,7 @@
         <v>63</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>98</v>
@@ -6479,7 +6459,7 @@
         <v>63</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E152" s="4" t="s">
         <v>98</v>
@@ -6504,7 +6484,7 @@
         <v>63</v>
       </c>
       <c r="D153" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>98</v>
@@ -6520,11 +6500,11 @@
     </row>
     <row r="154" spans="1:11" s="28" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A154" s="22" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B154" s="22"/>
       <c r="C154" s="22" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D154" s="23"/>
       <c r="E154" s="24" t="s">
@@ -6542,79 +6522,79 @@
       <c r="K154" s="27"/>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A155" s="49" t="s">
+      <c r="A155" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B155" s="49" t="s">
-        <v>373</v>
-      </c>
-      <c r="C155" s="49" t="s">
-        <v>372</v>
-      </c>
-      <c r="D155" s="50" t="s">
-        <v>376</v>
+      <c r="B155" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>374</v>
       </c>
       <c r="E155" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F155" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="G155" s="52"/>
-      <c r="H155" s="52"/>
-      <c r="I155" s="51"/>
-      <c r="J155" s="52"/>
-      <c r="K155" s="53"/>
+      <c r="F155" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G155" s="13"/>
+      <c r="H155" s="13"/>
+      <c r="I155" s="12"/>
+      <c r="J155" s="13"/>
+      <c r="K155" s="14"/>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A156" s="49" t="s">
+      <c r="A156" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B156" s="49" t="s">
-        <v>374</v>
-      </c>
-      <c r="C156" s="49" t="s">
+      <c r="B156" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="D156" s="50" t="s">
-        <v>377</v>
+      <c r="C156" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>375</v>
       </c>
       <c r="E156" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F156" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="G156" s="52"/>
-      <c r="H156" s="52"/>
-      <c r="I156" s="51"/>
-      <c r="J156" s="52"/>
-      <c r="K156" s="53"/>
+      <c r="F156" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G156" s="13"/>
+      <c r="H156" s="13"/>
+      <c r="I156" s="12"/>
+      <c r="J156" s="13"/>
+      <c r="K156" s="14"/>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A157" s="49" t="s">
+      <c r="A157" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B157" s="49" t="s">
-        <v>375</v>
-      </c>
-      <c r="C157" s="49" t="s">
-        <v>372</v>
-      </c>
-      <c r="D157" s="50" t="s">
-        <v>378</v>
+      <c r="B157" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>376</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F157" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="G157" s="52"/>
-      <c r="H157" s="52"/>
-      <c r="I157" s="51"/>
-      <c r="J157" s="52"/>
-      <c r="K157" s="53"/>
+      <c r="F157" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G157" s="13"/>
+      <c r="H157" s="13"/>
+      <c r="I157" s="12"/>
+      <c r="J157" s="13"/>
+      <c r="K157" s="14"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>

</xml_diff>